<commit_message>
finalizacion de carga de datos
</commit_message>
<xml_diff>
--- a/Base de datos/carga de datos.xlsx
+++ b/Base de datos/carga de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\techlogistic-4\techlogistic-4\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{070781F7-010C-4C7F-A420-F9484A15DBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0B7CFA-0F53-413F-B9A6-784BA55B1220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{75B10BB8-BD25-429E-A218-5692EA7C7360}"/>
+    <workbookView xWindow="-105" yWindow="2205" windowWidth="10455" windowHeight="7995" xr2:uid="{75B10BB8-BD25-429E-A218-5692EA7C7360}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>id_funcionario</t>
   </si>
@@ -85,13 +85,16 @@
   </si>
   <si>
     <t>piel de durazno</t>
+  </si>
+  <si>
+    <t>id_categoria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +104,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,13 +212,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD8041B-343C-4217-92ED-F64FA572D9A7}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +551,7 @@
     <col min="5" max="6" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,111 +564,138 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5">
-        <v>50000</v>
-      </c>
-      <c r="D2" s="5">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>540</v>
+      </c>
+      <c r="D3" s="3">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>540</v>
-      </c>
-      <c r="D3" s="4">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45350</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>64593453</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
+        <v>455690</v>
+      </c>
+      <c r="D6" s="3">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3450369</v>
+      </c>
+      <c r="D7" s="3">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
-        <v>45350</v>
-      </c>
-      <c r="D4" s="4">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4">
-        <v>64593453</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4">
-        <v>455690</v>
-      </c>
-      <c r="D6" s="4">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3450369</v>
-      </c>
-      <c r="D7" s="4">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>